<commit_message>
Done update, delete by excel
</commit_message>
<xml_diff>
--- a/public/template/Delete_BlackList_Template.xlsx
+++ b/public/template/Delete_BlackList_Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Pet Project\ip_manager\thaongu_ip_manager\public\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18B9FBCB-B8B6-441E-A3CC-7E49EA6F52DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0874DD43-9C5D-41C5-81AB-11D2EB25D658}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="810" yWindow="-120" windowWidth="23310" windowHeight="13740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
     <t>BlackList ID</t>
   </si>
   <si>
-    <t>_id</t>
+    <t>id</t>
   </si>
 </sst>
 </file>
@@ -385,7 +385,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>